<commit_message>
Ver QDS 0.4.1 Make Question View
</commit_message>
<xml_diff>
--- a/database/盈虧問題v3.xlsx
+++ b/database/盈虧問題v3.xlsx
@@ -34968,8 +34968,8 @@
   </sheetPr>
   <dimension ref="A1:H253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A228" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E253" activeCellId="0" sqref="A253:E253"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A238" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N253" activeCellId="0" sqref="N253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39268,6 +39268,12 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>